<commit_message>
Fixed holding import for Employee and Founder
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Last Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Founder or Employee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Instrument</t>
   </si>
   <si>
@@ -43,19 +46,46 @@
     <t xml:space="preserve">Emp1</t>
   </si>
   <si>
+    <t xml:space="preserve">Honest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Founder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emp2@mycompany.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emp2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emp3@mycompany.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awesome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Employee</t>
   </si>
   <si>
-    <t xml:space="preserve">Equity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emp2@mycompany.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emp2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preferred</t>
+    <t xml:space="preserve">emp4@mycompany.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super</t>
   </si>
 </sst>
 </file>
@@ -178,20 +208,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,64 +239,99 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="n">
+        <v>300</v>
+      </c>
       <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>400</v>
+      </c>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
@@ -277,6 +341,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
@@ -286,11 +351,14 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="emp1@mycompany.com"/>
     <hyperlink ref="A3" r:id="rId2" display="emp2@mycompany.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="emp3@mycompany.com"/>
+    <hyperlink ref="A5" r:id="rId4" display="emp4@mycompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Fixed import upload job for esop pool
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">Funding Round</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">Funding Round or ESOP Pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee ID</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
@@ -46,6 +49,9 @@
     <t xml:space="preserve">Price</t>
   </si>
   <si>
+    <t xml:space="preserve">Grant Date (mm/dd/yyyy)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Series A</t>
   </si>
   <si>
@@ -95,14 +101,21 @@
   </si>
   <si>
     <t xml:space="preserve">Super</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Options</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -186,7 +199,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +209,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,26 +234,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -257,142 +275,205 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>100</v>
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2345</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4567</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5678</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>9876</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="n">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>8765</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="n">
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="n">
+        <v>44470</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="emp1@mycompany.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="emp2@mycompany.com"/>
-    <hyperlink ref="B4" r:id="rId3" display="emp3@mycompany.com"/>
-    <hyperlink ref="B5" r:id="rId4" display="emp4@mycompany.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="emp1@mycompany.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="emp2@mycompany.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="emp3@mycompany.com"/>
+    <hyperlink ref="C5" r:id="rId4" display="emp4@mycompany.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="emp3@mycompany.com"/>
+    <hyperlink ref="C7" r:id="rId6" display="emp4@mycompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Renamed esop pool to option pool
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
-    <t xml:space="preserve">Funding Round or ESOP Pool</t>
+    <t xml:space="preserve">Funding Round or Option Pool</t>
   </si>
   <si>
     <t xml:space="preserve">Employee ID</t>
@@ -237,10 +237,10 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.14"/>

</xml_diff>

<commit_message>
Fixed tests for rename to option_pool
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t xml:space="preserve">Funding Round or Option Pool</t>
   </si>
@@ -106,7 +106,13 @@
     <t xml:space="preserve">Pool 1</t>
   </si>
   <si>
+    <t xml:space="preserve">emp5@mycompany.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emp6@mycompany.com</t>
   </si>
 </sst>
 </file>
@@ -237,7 +243,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -410,7 +416,7 @@
         <v>9876</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>21</v>
@@ -422,7 +428,7 @@
         <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>300</v>
@@ -442,7 +448,7 @@
         <v>8765</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>25</v>
@@ -454,7 +460,7 @@
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>400</v>
@@ -472,8 +478,8 @@
     <hyperlink ref="C3" r:id="rId2" display="emp2@mycompany.com"/>
     <hyperlink ref="C4" r:id="rId3" display="emp3@mycompany.com"/>
     <hyperlink ref="C5" r:id="rId4" display="emp4@mycompany.com"/>
-    <hyperlink ref="C6" r:id="rId5" display="emp3@mycompany.com"/>
-    <hyperlink ref="C7" r:id="rId6" display="emp4@mycompany.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="emp5@mycompany.com"/>
+    <hyperlink ref="C7" r:id="rId6" display="emp6@mycompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Pre creates vesting schedule for new option pool
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Investments" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Holdings" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -246,7 +246,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.14"/>

</xml_diff>

<commit_message>
Added document list to name for docs
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t xml:space="preserve">Funding Round or Option Pool</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Employee ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Department</t>
+  </si>
+  <si>
     <t xml:space="preserve">Email</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t xml:space="preserve">Series A</t>
   </si>
   <si>
+    <t xml:space="preserve">Tech</t>
+  </si>
+  <si>
     <t xml:space="preserve">emp1@mycompany.com</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
     <t xml:space="preserve">Equity</t>
   </si>
   <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
     <t xml:space="preserve">emp2@mycompany.com</t>
   </si>
   <si>
@@ -80,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Preferred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ops</t>
   </si>
   <si>
     <t xml:space="preserve">emp3@mycompany.com</t>
@@ -240,20 +252,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,7 +275,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -287,199 +299,220 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1234</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>100</v>
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2345</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4567</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
+      <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="J4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5678</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="J5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>9876</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="J6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="K6" s="3" t="n">
         <v>43915</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>8765</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="J7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="K7" s="3" t="n">
         <v>44470</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="emp1@mycompany.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="emp2@mycompany.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="emp3@mycompany.com"/>
-    <hyperlink ref="C5" r:id="rId4" display="emp4@mycompany.com"/>
-    <hyperlink ref="C6" r:id="rId5" display="emp5@mycompany.com"/>
-    <hyperlink ref="C7" r:id="rId6" display="emp6@mycompany.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="emp1@mycompany.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="emp2@mycompany.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="emp3@mycompany.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="emp4@mycompany.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="emp5@mycompany.com"/>
+    <hyperlink ref="D7" r:id="rId6" display="emp6@mycompany.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Added option type to holding
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t xml:space="preserve">Funding Round or Option Pool</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Instrument</t>
   </si>
   <si>
+    <t xml:space="preserve">Option Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
@@ -124,7 +127,13 @@
     <t xml:space="preserve">Options</t>
   </si>
   <si>
+    <t xml:space="preserve">Regular</t>
+  </si>
+  <si>
     <t xml:space="preserve">emp6@mycompany.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phantom</t>
   </si>
 </sst>
 </file>
@@ -252,20 +261,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,206 +311,219 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1234</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>100</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I2" s="1"/>
       <c r="J2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2345</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="K3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4567</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="K4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5678</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>9876</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="K6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="L6" s="3" t="n">
         <v>43915</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>8765</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="K7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="L7" s="3" t="n">
         <v>44470</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial version of holding conversion
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t xml:space="preserve">Funding Round or Option Pool</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Option Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred Conversion</t>
   </si>
   <si>
     <t xml:space="preserve">Quantity</t>
@@ -261,20 +264,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="24.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,216 +317,229 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1234</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="n">
-        <v>100</v>
-      </c>
+      <c r="J2" s="1"/>
       <c r="K2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2345</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="L3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4567</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="L4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5678</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>9876</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="L6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="M6" s="3" t="n">
         <v>43915</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>8765</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="K7" s="1" t="n">
+      <c r="L7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="M7" s="3" t="n">
         <v>44470</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Holding upload, does not create user verification email
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t xml:space="preserve">Funding Round or Option Pool</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
+    <t xml:space="preserve">Send Confirmation Email</t>
+  </si>
+  <si>
     <t xml:space="preserve">First Name</t>
   </si>
   <si>
@@ -67,7 +70,10 @@
     <t xml:space="preserve">Tech</t>
   </si>
   <si>
-    <t xml:space="preserve">emp1@mycompany.com</t>
+    <t xml:space="preserve">emp1@myfirm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">Emp1</t>
@@ -85,7 +91,7 @@
     <t xml:space="preserve">HR</t>
   </si>
   <si>
-    <t xml:space="preserve">emp2@mycompany.com</t>
+    <t xml:space="preserve">emp2@myfirm.com</t>
   </si>
   <si>
     <t xml:space="preserve">Emp2</t>
@@ -100,7 +106,7 @@
     <t xml:space="preserve">Ops</t>
   </si>
   <si>
-    <t xml:space="preserve">emp3@mycompany.com</t>
+    <t xml:space="preserve">emp3@myfirm.com</t>
   </si>
   <si>
     <t xml:space="preserve">Emp3</t>
@@ -112,7 +118,7 @@
     <t xml:space="preserve">Employee</t>
   </si>
   <si>
-    <t xml:space="preserve">emp4@mycompany.com</t>
+    <t xml:space="preserve">emp4@myfirm.com</t>
   </si>
   <si>
     <t xml:space="preserve">Emp4</t>
@@ -124,7 +130,10 @@
     <t xml:space="preserve">Pool 1</t>
   </si>
   <si>
-    <t xml:space="preserve">emp5@mycompany.com</t>
+    <t xml:space="preserve">emp5@myfirm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Options</t>
@@ -133,7 +142,7 @@
     <t xml:space="preserve">Regular</t>
   </si>
   <si>
-    <t xml:space="preserve">emp6@mycompany.com</t>
+    <t xml:space="preserve">emp6@myfirm.com</t>
   </si>
   <si>
     <t xml:space="preserve">Phantom</t>
@@ -264,20 +273,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -320,238 +329,251 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1234</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="n">
-        <v>100</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="N2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2345</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="n">
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="L3" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="M3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4567</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="M4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5678</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="n">
+      <c r="I5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="M5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>9876</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="M6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="N6" s="3" t="n">
         <v>43915</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>8765</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1" t="n">
+      <c r="J7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="M7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="N7" s="3" t="n">
         <v>44470</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="emp1@mycompany.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="emp2@mycompany.com"/>
-    <hyperlink ref="D4" r:id="rId3" display="emp3@mycompany.com"/>
-    <hyperlink ref="D5" r:id="rId4" display="emp4@mycompany.com"/>
-    <hyperlink ref="D6" r:id="rId5" display="emp5@mycompany.com"/>
-    <hyperlink ref="D7" r:id="rId6" display="emp6@mycompany.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added country code to IA
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25907E94-4243-4D4F-9E22-21BB4844636B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29D51C1-12CA-4F06-B094-320200AB5D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added tests for offers by investors
</commit_message>
<xml_diff>
--- a/public/sample_uploads/holdings.xlsx
+++ b/public/sample_uploads/holdings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29D51C1-12CA-4F06-B094-320200AB5D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F3D811-7E49-48B6-9DF9-92DB7AE2F20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>Funding Round or Option Pool</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Founder or Employee</t>
-  </si>
-  <si>
     <t>Instrument</t>
   </si>
   <si>
@@ -154,6 +151,30 @@
   </si>
   <si>
     <t>Grant Date (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Investor 1</t>
+  </si>
+  <si>
+    <t>Investor 2</t>
+  </si>
+  <si>
+    <t>Investor</t>
+  </si>
+  <si>
+    <t>emp1@investor1.com</t>
+  </si>
+  <si>
+    <t>emp1@investor2.com</t>
+  </si>
+  <si>
+    <t>Founder/Employee/Investor</t>
+  </si>
+  <si>
+    <t>Urban - Employees</t>
+  </si>
+  <si>
+    <t>Urban - Founders</t>
   </si>
 </sst>
 </file>
@@ -163,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -181,6 +202,14 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -201,17 +230,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -525,321 +561,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.19921875" customWidth="1"/>
-    <col min="2" max="4" width="24.1328125" customWidth="1"/>
-    <col min="5" max="6" width="50.6640625" customWidth="1"/>
-    <col min="7" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
-    <col min="15" max="15" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.19921875" customWidth="1"/>
+    <col min="3" max="5" width="24.1328125" customWidth="1"/>
+    <col min="6" max="7" width="50.6640625" customWidth="1"/>
+    <col min="8" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="14" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="16" max="16" width="22.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>1234</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>1234</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1">
-        <v>100</v>
-      </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1">
         <v>100</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="O2" s="1">
+        <v>100</v>
+      </c>
+      <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
         <v>2345</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1">
+        <v>200</v>
+      </c>
+      <c r="O3" s="1">
+        <v>100</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>4567</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1">
-        <v>2</v>
-      </c>
-      <c r="M3" s="1">
-        <v>200</v>
-      </c>
-      <c r="N3" s="1">
-        <v>100</v>
-      </c>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>4567</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1">
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
         <v>300</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>100</v>
       </c>
-      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>5678</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>5678</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1">
+        <v>400</v>
+      </c>
+      <c r="O5" s="1">
+        <v>100</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>9876</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
+        <v>300</v>
+      </c>
+      <c r="O6" s="1">
+        <v>10</v>
+      </c>
+      <c r="P6" s="3">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>8765</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <v>400</v>
+      </c>
+      <c r="O7" s="1">
+        <v>10</v>
+      </c>
+      <c r="P7" s="3">
+        <v>44470</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1">
-        <v>400</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="H8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="4">
         <v>100</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="O8" s="4">
+        <v>100</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6">
-        <v>9876</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1">
-        <v>300</v>
-      </c>
-      <c r="N6" s="1">
-        <v>10</v>
-      </c>
-      <c r="O6" s="3">
-        <v>43915</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7">
-        <v>8765</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
-        <v>400</v>
-      </c>
-      <c r="N7" s="1">
-        <v>10</v>
-      </c>
-      <c r="O7" s="3">
-        <v>44470</v>
+    <row r="9" spans="1:16" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="4">
+        <v>200</v>
+      </c>
+      <c r="O9" s="4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{0C155EE1-6B52-462E-B6B4-7951D59486F0}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{7B0DEB66-EF5F-424D-88E3-23A712292985}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{25D95E5D-C3C2-47E4-BB9C-8A919574F893}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>